<commit_message>
Added archive backup file.
</commit_message>
<xml_diff>
--- a/notes/nthroot/bundles.xlsx
+++ b/notes/nthroot/bundles.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E6C41A-DCE4-4034-95B4-70C71F967DF8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A31BE2-65EA-4C7A-84CD-431DCDBAE54B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nthRoot3" sheetId="1" r:id="rId1"/>
     <sheet name="nthRoot4" sheetId="2" r:id="rId2"/>
     <sheet name="nthRoot9" sheetId="3" r:id="rId3"/>
+    <sheet name="nthRoot9-2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>Largest Multiple of nth root less than or equal to magnitude</t>
   </si>
@@ -100,6 +101,18 @@
   </si>
   <si>
     <t>Magnitude less than nthRoot divide by 10^0</t>
+  </si>
+  <si>
+    <t>Quo =</t>
+  </si>
+  <si>
+    <t>Mod =</t>
+  </si>
+  <si>
+    <t>mod =</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = bundle 2</t>
   </si>
 </sst>
 </file>
@@ -458,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D6:F27"/>
+  <dimension ref="D6:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,12 +482,12 @@
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D7" s="3">
         <v>3</v>
       </c>
@@ -482,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D8" s="1">
         <v>98327123</v>
       </c>
@@ -490,23 +503,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D9" s="3">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D10" s="3">
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
@@ -514,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D13" s="3">
         <f>D8/POWER(10,6)</f>
         <v>98.327123</v>
@@ -523,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="4:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D15" s="5">
         <v>98</v>
       </c>
@@ -630,10 +667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A7253D-47AB-4549-AA1B-96639CB1F79F}">
-  <dimension ref="D3:F16"/>
+  <dimension ref="D3:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +678,7 @@
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D3" s="3">
         <v>4</v>
       </c>
@@ -649,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D4" s="1">
         <v>98327123</v>
       </c>
@@ -657,23 +694,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D5" s="3">
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D6" s="3">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D7" s="4" t="s">
         <v>18</v>
       </c>
@@ -681,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D8" s="3">
         <f>D4/POWER(10,4)</f>
         <v>9832.7122999999992</v>
@@ -690,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D9" s="5">
         <v>9832</v>
       </c>
@@ -699,7 +760,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="11" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D11" s="3">
         <v>7123</v>
       </c>
@@ -707,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D12" s="3">
         <v>3</v>
       </c>
@@ -715,7 +776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
@@ -723,7 +784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D14" s="3">
         <f>D11/POWER(10,0)</f>
         <v>7123</v>
@@ -732,7 +793,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="5">
+        <v>7123</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D16" s="3">
         <v>0</v>
       </c>
@@ -749,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDAB58E-8FDE-41DE-BD0D-5DD08E2884E4}">
   <dimension ref="C3:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,4 +919,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7C97A5-19D5-400D-884D-AC3B02725D6F}">
+  <dimension ref="C3:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1">
+        <v>983271230</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="3">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3">
+        <f>C4/POWER(10,0)</f>
+        <v>983271230</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="3">
+        <v>983271230</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="13" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working Version of BigIntMathNthRoot.
</commit_message>
<xml_diff>
--- a/notes/nthroot/bundles.xlsx
+++ b/notes/nthroot/bundles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38085E47-3B76-41B4-884A-A6DE4E804BF0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AA6B50-6E1C-46D4-A611-FE2CBCFB16F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="113">
   <si>
     <t>Largest Multiple of nth root less than or equal to magnitude</t>
   </si>
@@ -326,6 +326,51 @@
   </si>
   <si>
     <t>8.03541479949853</t>
+  </si>
+  <si>
+    <t>Quotient</t>
+  </si>
+  <si>
+    <t>264.567</t>
+  </si>
+  <si>
+    <t>16.265516</t>
+  </si>
+  <si>
+    <t>2 64 56</t>
+  </si>
+  <si>
+    <t>2 64 5</t>
+  </si>
+  <si>
+    <t>98 327 123</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>64 5</t>
+  </si>
+  <si>
+    <t>8.031189</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Frac</t>
+  </si>
+  <si>
+    <t>64 56</t>
+  </si>
+  <si>
+    <t>64 56 7</t>
+  </si>
+  <si>
+    <t>Int Bundle</t>
+  </si>
+  <si>
+    <t>Mod</t>
   </si>
 </sst>
 </file>
@@ -385,7 +430,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,7 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -417,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,14 +508,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -777,683 +828,989 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A08185-BBB3-48F3-82F6-785099575CF7}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J1" s="27" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F2" s="25"/>
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="Q2" s="26"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
         <v>65</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
         <v>73</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N3" t="s">
         <v>81</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O3" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="P2" s="21"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="Q3" s="25"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="21"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="25">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="9">
+        <f>QUOTIENT(N4,E4)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <f>MOD(N4,E4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <f>H4+IF(I4&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="9">
+        <f>QUOTIENT(O4,E4)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <f>+K4+J4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="25">
+        <v>1</v>
+      </c>
+      <c r="N4" s="25">
+        <v>2</v>
+      </c>
+      <c r="O4" s="25">
+        <v>1</v>
+      </c>
+      <c r="P4" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>1+A4</f>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="21">
+      <c r="D5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="21">
         <v>31</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <f>+I3+H3</f>
+      <c r="H5" s="9">
+        <f t="shared" ref="H5:H19" si="0">QUOTIENT(N5,E5)</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" ref="I5:I19" si="1">MOD(N5,E5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J19" si="2">H5+IF(I5&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" ref="K5:K19" si="3">QUOTIENT(O5,E5)</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" ref="L5:L19" si="4">+K5+J5</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="29">
+        <v>2</v>
+      </c>
+      <c r="N5" s="25">
+        <v>2</v>
+      </c>
+      <c r="O5" s="25">
+        <v>2</v>
+      </c>
+      <c r="P5" s="25">
+        <f>+O5+N5</f>
         <v>4</v>
       </c>
-      <c r="K3">
-        <f>QUOTIENT(J3,D3)</f>
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <f>IF(MOD(J3,D3) &gt; 0,1,0)</f>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>1+A5</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>14</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M3">
-        <f>+L3+K3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>1+A3</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="21">
+      <c r="J6" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="M6" s="29">
+        <v>2</v>
+      </c>
+      <c r="N6" s="25">
+        <v>2</v>
+      </c>
+      <c r="O6" s="25">
+        <v>3</v>
+      </c>
+      <c r="P6" s="25">
+        <f>+O6+N6</f>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ref="A7:A16" si="5">1+A6</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="21">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="9">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <f>+I4+H4</f>
+      <c r="G7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M7" s="29">
+        <v>3</v>
+      </c>
+      <c r="N7" s="25">
+        <v>2</v>
+      </c>
+      <c r="O7" s="25">
+        <v>4</v>
+      </c>
+      <c r="P7" s="25">
+        <f>+O7+N7</f>
+        <v>6</v>
+      </c>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="K4">
-        <f>QUOTIENT(J4,D4)</f>
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <f>IF(MOD(J4,D4) &gt; 0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="25">
-        <f>+L4+K4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" ref="A5:A9" si="0">1+A4</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="C8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21">
         <v>14</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="9">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
+      <c r="G8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L8" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M8" s="29">
+        <v>3</v>
+      </c>
+      <c r="N8" s="25">
+        <v>2</v>
+      </c>
+      <c r="O8" s="25">
         <v>4</v>
       </c>
-      <c r="J5">
-        <f>+I5+H5</f>
+      <c r="P8" s="25">
+        <f>+O8+N8</f>
         <v>6</v>
       </c>
-      <c r="K5">
-        <f>QUOTIENT(J5,D5)</f>
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <f>IF(MOD(J5,D5) &gt; 0,1,0)</f>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21">
+        <v>14</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M5">
-        <f>+L5+K5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="J9" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L9" s="9">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M9" s="29">
+        <v>4</v>
+      </c>
+      <c r="N9" s="25">
+        <v>2</v>
+      </c>
+      <c r="O9" s="25">
+        <v>6</v>
+      </c>
+      <c r="P9" s="25">
+        <f>+O9+N9</f>
+        <v>8</v>
+      </c>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="21">
+        <v>14</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="21">
-        <v>14</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" s="9">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <f>+I6+H6</f>
-        <v>6</v>
-      </c>
-      <c r="K6">
-        <f>QUOTIENT(J6,D6)</f>
-        <v>3</v>
-      </c>
-      <c r="L6">
-        <f>IF(MOD(J6,D6) &gt; 0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6">
-        <f>+L6+K6</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" s="21">
-        <v>14</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="9">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <f>+I7+H7</f>
-        <v>8</v>
-      </c>
-      <c r="K7">
-        <f>QUOTIENT(J7,D7)</f>
-        <v>4</v>
-      </c>
-      <c r="L7">
-        <f>IF(MOD(J7,D7) &gt; 0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f>+L7+K7</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="21">
-        <v>14</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J16" si="1">+I8+H8</f>
-        <v>3</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ref="K8:K16" si="2">QUOTIENT(J8,D8)</f>
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <f t="shared" ref="L8:L16" si="3">IF(MOD(J8,D8) &gt; 0,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="25">
-        <f t="shared" ref="M8:M16" si="4">+L8+K8</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="22">
-        <v>64</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="21">
-        <v>6</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K9">
+      <c r="J10" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="K10" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9">
+      <c r="L10" s="9">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" ref="A10:A16" si="5">1+A9</f>
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="21">
-        <v>6</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M10" s="29">
+        <v>1</v>
+      </c>
+      <c r="N10" s="25">
+        <v>2</v>
+      </c>
+      <c r="O10" s="25">
+        <v>1</v>
+      </c>
+      <c r="P10" s="25">
+        <f t="shared" ref="P10:P19" si="6">+O10+N10</f>
+        <v>3</v>
+      </c>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="24">
-        <v>264.56</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="21">
-        <v>14</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="22">
+        <v>64</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="21">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L11">
+      <c r="K11" s="9">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M11" s="25">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N11" s="25">
+        <v>2</v>
+      </c>
+      <c r="O11" s="25">
+        <v>0</v>
+      </c>
+      <c r="P11" s="25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="22">
         <v>264.5</v>
       </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="21">
+      <c r="D12" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="21">
         <v>6</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="L12">
+      <c r="K12" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="L12" s="9">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M12" s="25">
+        <v>2</v>
+      </c>
+      <c r="N12" s="25">
+        <v>3</v>
+      </c>
+      <c r="O12" s="25">
+        <v>1</v>
+      </c>
+      <c r="P12" s="25">
+        <f>+O12+N12</f>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="22">
-        <v>264.5</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" s="21">
-        <v>14</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="21">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="K13" s="9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="L13" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
       <c r="M13" s="25">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="N13" s="25">
+        <v>3</v>
+      </c>
+      <c r="O13" s="25">
+        <v>2</v>
+      </c>
+      <c r="P13" s="25">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="Q13" s="25"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="25">
+        <v>6</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M14" s="25">
+        <v>3</v>
+      </c>
+      <c r="N14" s="25">
+        <v>3</v>
+      </c>
+      <c r="O14" s="25">
+        <v>3</v>
+      </c>
+      <c r="P14" s="25">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="Q14" s="25"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" s="21">
-        <v>12</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14">
+      <c r="C15" s="24">
+        <v>264.56</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="21">
+        <v>14</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="9">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="L15" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M15" s="25">
+        <v>1</v>
+      </c>
+      <c r="N15" s="25">
+        <v>3</v>
+      </c>
+      <c r="O15" s="25">
+        <v>2</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="C16" s="22">
+        <v>264.5</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" s="21">
+        <v>14</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="25">
+        <v>1</v>
+      </c>
+      <c r="N16" s="25">
+        <v>3</v>
+      </c>
+      <c r="O16" s="25">
+        <v>1</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ref="A17:A19" si="7">1+A16</f>
+        <v>14</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="21">
+        <v>12</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K17" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="9">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="5"/>
+      <c r="M17" s="25">
+        <v>4</v>
+      </c>
+      <c r="N17" s="25">
+        <v>5</v>
+      </c>
+      <c r="O17" s="25">
+        <v>3</v>
+      </c>
+      <c r="P17" s="25">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" s="21">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="G18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K18" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M18" s="25">
+        <v>3</v>
+      </c>
+      <c r="N18" s="25">
+        <v>5</v>
+      </c>
+      <c r="O18" s="25">
+        <v>3</v>
+      </c>
+      <c r="P18" s="25">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" s="21">
+      <c r="D19" s="9"/>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" s="21">
         <v>13</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15">
+      <c r="G19" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" s="21">
-        <v>13</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>5</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L16">
+      <c r="K19" s="9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M16">
+      <c r="L19" s="9">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
+      <c r="M19" s="25">
+        <v>2</v>
+      </c>
+      <c r="N19" s="25">
+        <v>5</v>
+      </c>
+      <c r="O19" s="25">
+        <v>3</v>
+      </c>
+      <c r="P19" s="25">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Q19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Last working version before adding fractional leading zeros routine.
</commit_message>
<xml_diff>
--- a/notes/nthroot/bundles.xlsx
+++ b/notes/nthroot/bundles.xlsx
@@ -3,28 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DE32C1-F5CA-4150-892E-0C3D58901E86}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8493C8-4916-471A-BD79-FA0CE4A57760}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrialRuns" sheetId="12" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="15" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="17" r:id="rId4"/>
+    <sheet name="bundles1" sheetId="14" r:id="rId2"/>
+    <sheet name="bundles2" sheetId="15" r:id="rId3"/>
+    <sheet name="bundles3" sheetId="17" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="16" r:id="rId5"/>
     <sheet name="nthRoot3" sheetId="1" r:id="rId6"/>
-    <sheet name="nthRoot4" sheetId="2" r:id="rId7"/>
-    <sheet name="nthRoot9" sheetId="3" r:id="rId8"/>
-    <sheet name="nthRoot9-2" sheetId="4" r:id="rId9"/>
+    <sheet name="nthRoot3-2" sheetId="18" r:id="rId7"/>
+    <sheet name="nthRoot4" sheetId="2" r:id="rId8"/>
+    <sheet name="nthRoot4-2" sheetId="11" r:id="rId9"/>
     <sheet name="nthRoot2-4" sheetId="10" r:id="rId10"/>
-    <sheet name="nthRoot3-2" sheetId="11" r:id="rId11"/>
-    <sheet name="precision-1" sheetId="5" r:id="rId12"/>
-    <sheet name="precision-2" sheetId="6" r:id="rId13"/>
-    <sheet name="precision-3" sheetId="7" r:id="rId14"/>
-    <sheet name="precision-4" sheetId="8" r:id="rId15"/>
-    <sheet name="precision-5" sheetId="9" r:id="rId16"/>
-    <sheet name="precision-6" sheetId="13" r:id="rId17"/>
+    <sheet name="nthRoot9" sheetId="3" r:id="rId11"/>
+    <sheet name="nthRoot9-2" sheetId="4" r:id="rId12"/>
+    <sheet name="precision-1" sheetId="5" r:id="rId13"/>
+    <sheet name="precision-2" sheetId="6" r:id="rId14"/>
+    <sheet name="precision-3" sheetId="7" r:id="rId15"/>
+    <sheet name="precision-4" sheetId="8" r:id="rId16"/>
+    <sheet name="precision-5" sheetId="9" r:id="rId17"/>
+    <sheet name="precision-6" sheetId="13" r:id="rId18"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="144">
   <si>
     <t>Largest Multiple of nth root less than or equal to magnitude</t>
   </si>
@@ -438,13 +439,43 @@
   </si>
   <si>
     <t>Bundle-3</t>
+  </si>
+  <si>
+    <t>Multiplier = Magnitude / nthRoot</t>
+  </si>
+  <si>
+    <t>Exponent = nthRoot X Multiplier</t>
+  </si>
+  <si>
+    <t>ScaleVal = 10^Exponent</t>
+  </si>
+  <si>
+    <t>Bundle = Quotient (Radicand / ScaleVal)</t>
+  </si>
+  <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>Bundle 2</t>
+  </si>
+  <si>
+    <t>Bundle 3</t>
+  </si>
+  <si>
+    <t>INTEGER DIGITS</t>
+  </si>
+  <si>
+    <t>Leading Zeros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Magnitude = Magnitude + Leading Zeros </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
@@ -454,6 +485,7 @@
     <numFmt numFmtId="170" formatCode="0.00000"/>
     <numFmt numFmtId="171" formatCode="0.00000000"/>
     <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -554,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -635,10 +667,11 @@
     <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -968,8 +1001,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
       <c r="U1" s="25"/>
       <c r="V1" s="25"/>
     </row>
@@ -2026,156 +2059,201 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC11DC1B-2CEC-4FBC-ADD7-73CA61C21010}">
-  <dimension ref="D3:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDAB58E-8FDE-41DE-BD0D-5DD08E2884E4}">
+  <dimension ref="C3:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D3" s="3">
+    <row r="3" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D4" s="1">
+    </row>
+    <row r="4" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1">
         <v>98327123</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D5" s="3">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C5" s="3">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D6" s="3">
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="3">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D8" s="3">
-        <f>D4/POWER(10,4)</f>
-        <v>9832.7122999999992</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D9" s="5">
-        <v>9832</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="3">
+        <f>+C4*POWER(10,1)</f>
+        <v>983271230</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="3">
         <v>8</v>
       </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="11" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D11" s="3">
-        <v>7123</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C12" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D14" s="3">
-        <f>D11/POWER(10,0)</f>
-        <v>7123</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D15" s="5">
-        <v>7123</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C14" s="2">
+        <f>+C10/POWER(10,0)</f>
+        <v>983271230</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7C97A5-19D5-400D-884D-AC3B02725D6F}">
+  <dimension ref="C3:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1">
+        <v>983271230</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="3">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3">
+        <f>C4/POWER(10,0)</f>
+        <v>983271230</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C11" s="3">
+        <v>983271230</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="13" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F5DF80-EF70-4B4D-A7D6-0733E2C43353}">
   <dimension ref="E3:Q17"/>
   <sheetViews>
@@ -2382,12 +2460,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C28F389-1331-4051-83F6-10A5A26D1AF9}">
   <dimension ref="C2:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104113D6-5DBA-41D8-9C7E-09EB1EAA3D3E}">
   <dimension ref="C2:P16"/>
   <sheetViews>
@@ -2834,7 +2912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38E82AD-C86B-4FB6-B5D0-72FCD37FF65F}">
   <dimension ref="C2:Q16"/>
   <sheetViews>
@@ -3065,7 +3143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1CD97A-6BF1-46E9-B4A0-3A5C60052C42}">
   <dimension ref="C2:S17"/>
   <sheetViews>
@@ -3298,7 +3376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0DCCEE-B346-4930-A2C9-A289DE597159}">
   <dimension ref="C2:S18"/>
   <sheetViews>
@@ -3543,7 +3621,7 @@
   <dimension ref="A4:X150"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="P101" sqref="P101:U103"/>
+      <selection activeCell="P101" sqref="P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,7 +7226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9576092-BB4F-46E4-9212-F39310F079AD}">
   <dimension ref="B2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -7169,20 +7247,20 @@
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="2:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="C4" s="45">
-        <v>1</v>
-      </c>
-      <c r="F4" s="45">
-        <v>0</v>
-      </c>
-      <c r="G4" s="45">
-        <v>0</v>
-      </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45">
+      <c r="C4" s="44">
+        <v>1</v>
+      </c>
+      <c r="F4" s="44">
+        <v>0</v>
+      </c>
+      <c r="G4" s="44">
+        <v>0</v>
+      </c>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44">
         <v>6</v>
       </c>
-      <c r="J4" s="45">
+      <c r="J4" s="44">
         <v>5</v>
       </c>
     </row>
@@ -8295,7 +8373,7 @@
   <dimension ref="D6:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8487,11 +8565,783 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386B31B5-45E2-49C7-813A-756A8E1563AE}">
+  <dimension ref="C3:T82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71:T71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D3" s="8">
+        <v>98327654.122999996</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D4" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="3">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D16" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="T16" s="3">
+        <f>QUOTIENT(D17,$D$6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D17" s="3">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="T17" s="3">
+        <f>$D$6*T16</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D18" s="3">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="T18" s="1">
+        <f>POWER(10,T17)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D19" s="3">
+        <f>+T19</f>
+        <v>98</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T19" s="3">
+        <f>QUOTIENT(D16,T18)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D21" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D22" s="1">
+        <v>327654</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="T22" s="3">
+        <f>QUOTIENT(D23,$D$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="T23" s="3">
+        <f>$D$6*T22</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N24" s="12"/>
+      <c r="T24" s="1">
+        <f>POWER(10,T23)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D25" s="3">
+        <f>+T25</f>
+        <v>327</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T25" s="3">
+        <f>QUOTIENT(D22,T24)</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D27" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D28" s="1">
+        <v>654</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="T28" s="3">
+        <f>QUOTIENT(D29,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="T29" s="3">
+        <f>$D$6*T28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="T30" s="1">
+        <f>POWER(10,T29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D31" s="3">
+        <f>+T31</f>
+        <v>654</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T31" s="3">
+        <f>QUOTIENT(D28,T30)</f>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C33" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="35" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D35" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D36" s="1">
+        <v>123</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="T36" s="3">
+        <f>QUOTIENT(D37,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="T37" s="3">
+        <f>$D$6*T36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="T38" s="1">
+        <f>POWER(10,T37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D39" s="3">
+        <f>+T39</f>
+        <v>123</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T39" s="3">
+        <f>QUOTIENT(D36,T38)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D44" s="46">
+        <v>98000054.000012293</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D45" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D46" s="1">
+        <v>123</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D48" s="3">
+        <v>7</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D49" s="3">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C51" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D52" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D53" s="3">
+        <v>7</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D54" s="3">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D56" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D57" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N57" s="3"/>
+      <c r="T57" s="3">
+        <f>QUOTIENT(D58,$D$6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="3">
+        <v>7</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N58" s="3"/>
+      <c r="T58" s="3">
+        <f>$D$6*T57</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D59" s="3">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N59" s="12"/>
+      <c r="T59" s="1">
+        <f>POWER(10,T58)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="60" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D60" s="3">
+        <f>+T60</f>
+        <v>98</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T60" s="3">
+        <f>QUOTIENT(D57,T59)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D62" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D63" s="1">
+        <v>54</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="T63" s="1">
+        <f>+D65+D64</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D64" s="1">
+        <v>4</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N64" s="3"/>
+      <c r="T64" s="3">
+        <f>QUOTIENT(D65,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N65" s="3"/>
+      <c r="T65" s="3">
+        <f>$D$6*T64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D66" s="3">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N66" s="12"/>
+      <c r="T66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D69" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D70" s="1">
+        <v>54</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N71" s="3"/>
+      <c r="T71" s="3">
+        <f>QUOTIENT(D72,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D72" s="3">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N72" s="3"/>
+      <c r="T72" s="3">
+        <f>$D$6*T71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D73" s="3">
+        <v>3</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N73" s="12"/>
+      <c r="T73" s="1">
+        <f>POWER(10,T72)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D74" s="3">
+        <f>+T74</f>
+        <v>54</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T74" s="3">
+        <f>QUOTIENT(D70,T73)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C76" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="78" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D78" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D79" s="1">
+        <v>123</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N79" s="3"/>
+      <c r="T79" s="3">
+        <f>QUOTIENT(D80,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D80" s="3">
+        <v>2</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N80" s="3"/>
+      <c r="T80" s="3">
+        <f>$D$6*T79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D81" s="3">
+        <v>3</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N81" s="12"/>
+      <c r="T81" s="1">
+        <f>POWER(10,T80)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D82" s="3">
+        <f>+T82</f>
+        <v>123</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T82" s="3">
+        <f>QUOTIENT(D79,T81)</f>
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A7253D-47AB-4549-AA1B-96639CB1F79F}">
   <dimension ref="D3:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8636,197 +9486,152 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDAB58E-8FDE-41DE-BD0D-5DD08E2884E4}">
-  <dimension ref="C3:D14"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC11DC1B-2CEC-4FBC-ADD7-73CA61C21010}">
+  <dimension ref="D3:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C3" s="3">
+    <row r="3" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D4" s="1">
+        <v>98327123</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D6" s="3">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="3">
+        <f>D4/POWER(10,4)</f>
+        <v>9832.7122999999992</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D9" s="5">
+        <v>9832</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="11" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="3">
+        <v>7123</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="1">
-        <v>98327123</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C5" s="3">
+    </row>
+    <row r="12" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D14" s="3">
+        <f>D11/POWER(10,0)</f>
+        <v>7123</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C6" s="3">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C10" s="3">
-        <f>+C4*POWER(10,1)</f>
-        <v>983271230</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C11" s="3">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C12" s="3">
-        <v>9</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C14" s="2">
-        <f>+C10/POWER(10,0)</f>
-        <v>983271230</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
+    </row>
+    <row r="15" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="5">
+        <v>7123</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="4:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7C97A5-19D5-400D-884D-AC3B02725D6F}">
-  <dimension ref="C3:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C3" s="3">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="1">
-        <v>983271230</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C5" s="3">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C6" s="3">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C9" s="3">
-        <f>C4/POWER(10,0)</f>
-        <v>983271230</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C11" s="3">
-        <v>983271230</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="13" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated bundles spreadsheet notes.
</commit_message>
<xml_diff>
--- a/notes/nthroot/bundles.xlsx
+++ b/notes/nthroot/bundles.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8493C8-4916-471A-BD79-FA0CE4A57760}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E255C7-82EE-4E97-B81B-7A4F5C3DDAE6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrialRuns" sheetId="12" r:id="rId1"/>
@@ -17,15 +17,16 @@
     <sheet name="nthRoot3-2" sheetId="18" r:id="rId7"/>
     <sheet name="nthRoot4" sheetId="2" r:id="rId8"/>
     <sheet name="nthRoot4-2" sheetId="11" r:id="rId9"/>
-    <sheet name="nthRoot2-4" sheetId="10" r:id="rId10"/>
-    <sheet name="nthRoot9" sheetId="3" r:id="rId11"/>
-    <sheet name="nthRoot9-2" sheetId="4" r:id="rId12"/>
-    <sheet name="precision-1" sheetId="5" r:id="rId13"/>
-    <sheet name="precision-2" sheetId="6" r:id="rId14"/>
-    <sheet name="precision-3" sheetId="7" r:id="rId15"/>
-    <sheet name="precision-4" sheetId="8" r:id="rId16"/>
-    <sheet name="precision-5" sheetId="9" r:id="rId17"/>
-    <sheet name="precision-6" sheetId="13" r:id="rId18"/>
+    <sheet name="nthRoot5-1" sheetId="19" r:id="rId10"/>
+    <sheet name="nthRoot2-4" sheetId="10" r:id="rId11"/>
+    <sheet name="nthRoot9" sheetId="3" r:id="rId12"/>
+    <sheet name="nthRoot9-2" sheetId="4" r:id="rId13"/>
+    <sheet name="precision-1" sheetId="5" r:id="rId14"/>
+    <sheet name="precision-2" sheetId="6" r:id="rId15"/>
+    <sheet name="precision-3" sheetId="7" r:id="rId16"/>
+    <sheet name="precision-4" sheetId="8" r:id="rId17"/>
+    <sheet name="precision-5" sheetId="9" r:id="rId18"/>
+    <sheet name="precision-6" sheetId="13" r:id="rId19"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="146">
   <si>
     <t>Largest Multiple of nth root less than or equal to magnitude</t>
   </si>
@@ -469,6 +470,12 @@
   </si>
   <si>
     <t xml:space="preserve">Actual Magnitude = Magnitude + Leading Zeros </t>
+  </si>
+  <si>
+    <t>Remainder</t>
+  </si>
+  <si>
+    <t>Radicand - (ScaleVal X Bundle)</t>
   </si>
 </sst>
 </file>
@@ -668,10 +675,10 @@
     <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1001,8 +1008,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
       <c r="U1" s="25"/>
       <c r="V1" s="25"/>
     </row>
@@ -1971,6 +1978,804 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE433CDA-DA93-4ADC-87D0-0C6CD5FAD8A2}">
+  <dimension ref="C3:T84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D3" s="8">
+        <v>5604423.9239999996</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D4" s="1">
+        <v>5604423</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D5" s="1">
+        <v>924</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="3">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="1">
+        <v>5604423</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D16" s="1">
+        <v>5604423</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="T16" s="3">
+        <f>QUOTIENT(D17,$D$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D17" s="3">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="T17" s="3">
+        <f>$D$6*T16</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D18" s="3">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="T18" s="1">
+        <f>POWER(10,T17)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D19" s="3">
+        <f>+T19</f>
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T19" s="3">
+        <f>QUOTIENT(D16,T18)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D20" s="3">
+        <f>+T20</f>
+        <v>4423</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="T20" s="3">
+        <f>+D16-(T19*T18)</f>
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="23" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D23" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D24" s="1">
+        <v>327654</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="T24" s="3">
+        <f>QUOTIENT(D25,$D$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D25" s="3">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="T25" s="3">
+        <f>$D$6*T24</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D26" s="3">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N26" s="12"/>
+      <c r="T26" s="1">
+        <f>POWER(10,T25)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="27" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D27" s="3">
+        <f>+T27</f>
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T27" s="3">
+        <f>QUOTIENT(D24,T26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D29" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D30" s="1">
+        <v>654</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="T30" s="3">
+        <f>QUOTIENT(D31,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="T31" s="3">
+        <f>$D$6*T30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N32" s="12"/>
+      <c r="T32" s="1">
+        <f>POWER(10,T31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D33" s="3">
+        <f>+T33</f>
+        <v>654</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T33" s="3">
+        <f>QUOTIENT(D30,T32)</f>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="37" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D37" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D38" s="1">
+        <v>123</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="T38" s="3">
+        <f>QUOTIENT(D39,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N39" s="3"/>
+      <c r="T39" s="3">
+        <f>$D$6*T38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N40" s="12"/>
+      <c r="T40" s="1">
+        <f>POWER(10,T39)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D41" s="3">
+        <f>+T41</f>
+        <v>123</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T41" s="3">
+        <f>QUOTIENT(D38,T40)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D46" s="45">
+        <v>98000054.000012293</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D47" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D48" s="1">
+        <v>123</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D49" s="1">
+        <v>3</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D50" s="3">
+        <v>7</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D51" s="3">
+        <v>7</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C53" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D54" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D55" s="3">
+        <v>7</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D56" s="3">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D59" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N59" s="3"/>
+      <c r="T59" s="3">
+        <f>QUOTIENT(D60,$D$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D60" s="3">
+        <v>7</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N60" s="3"/>
+      <c r="T60" s="3">
+        <f>$D$6*T59</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D61" s="3">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N61" s="12"/>
+      <c r="T61" s="1">
+        <f>POWER(10,T60)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="62" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D62" s="3">
+        <f>+T62</f>
+        <v>980</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T62" s="3">
+        <f>QUOTIENT(D59,T61)</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="64" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D64" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D65" s="1">
+        <v>54</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="T65" s="1">
+        <f>+D67+D66</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D66" s="1">
+        <v>4</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N66" s="3"/>
+      <c r="T66" s="3">
+        <f>QUOTIENT(D67,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D67" s="3">
+        <v>1</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N67" s="3"/>
+      <c r="T67" s="3">
+        <f>$D$6*T66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D68" s="3">
+        <v>2</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N68" s="12"/>
+      <c r="T68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D71" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D72" s="1">
+        <v>54</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N73" s="3"/>
+      <c r="T73" s="3">
+        <f>QUOTIENT(D74,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D74" s="3">
+        <v>2</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N74" s="3"/>
+      <c r="T74" s="3">
+        <f>$D$6*T73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D75" s="3">
+        <v>3</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L75" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N75" s="12"/>
+      <c r="T75" s="1">
+        <f>POWER(10,T74)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D76" s="3">
+        <f>+T76</f>
+        <v>54</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T76" s="3">
+        <f>QUOTIENT(D72,T75)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C78" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="80" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D80" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D81" s="1">
+        <v>123</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N81" s="3"/>
+      <c r="T81" s="3">
+        <f>QUOTIENT(D82,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D82" s="3">
+        <v>2</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N82" s="3"/>
+      <c r="T82" s="3">
+        <f>$D$6*T81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D83" s="3">
+        <v>3</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N83" s="12"/>
+      <c r="T83" s="1">
+        <f>POWER(10,T82)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D84" s="3">
+        <f>+T84</f>
+        <v>123</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T84" s="3">
+        <f>QUOTIENT(D81,T83)</f>
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03409A07-B58B-490F-BED8-8C6B21724E03}">
   <dimension ref="C3:E14"/>
   <sheetViews>
@@ -2058,7 +2863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDAB58E-8FDE-41DE-BD0D-5DD08E2884E4}">
   <dimension ref="C3:D14"/>
   <sheetViews>
@@ -2164,7 +2969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7C97A5-19D5-400D-884D-AC3B02725D6F}">
   <dimension ref="C3:E14"/>
   <sheetViews>
@@ -2253,7 +3058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F5DF80-EF70-4B4D-A7D6-0733E2C43353}">
   <dimension ref="E3:Q17"/>
   <sheetViews>
@@ -2460,7 +3265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C28F389-1331-4051-83F6-10A5A26D1AF9}">
   <dimension ref="C2:O16"/>
   <sheetViews>
@@ -2678,7 +3483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104113D6-5DBA-41D8-9C7E-09EB1EAA3D3E}">
   <dimension ref="C2:P16"/>
   <sheetViews>
@@ -2912,7 +3717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38E82AD-C86B-4FB6-B5D0-72FCD37FF65F}">
   <dimension ref="C2:Q16"/>
   <sheetViews>
@@ -3143,7 +3948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1CD97A-6BF1-46E9-B4A0-3A5C60052C42}">
   <dimension ref="C2:S17"/>
   <sheetViews>
@@ -3376,7 +4181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0DCCEE-B346-4930-A2C9-A289DE597159}">
   <dimension ref="C2:S18"/>
   <sheetViews>
@@ -8568,8 +9373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386B31B5-45E2-49C7-813A-756A8E1563AE}">
   <dimension ref="C3:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71:T71"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8945,7 +9750,7 @@
       </c>
     </row>
     <row r="44" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D44" s="46">
+      <c r="D44" s="45">
         <v>98000054.000012293</v>
       </c>
       <c r="E44" s="3" t="s">

</xml_diff>

<commit_message>
Refactored BigIntMathNthRoot.getNextBundle() for intExpectedActualDelta comparison to nthRoot.
</commit_message>
<xml_diff>
--- a/notes/nthroot/bundles.xlsx
+++ b/notes/nthroot/bundles.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F915B61-A92B-4988-9773-5EE8D7FEC5B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A61454B-08E3-432A-8D0B-8BD099B0AC0F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TrialRuns" sheetId="12" r:id="rId1"/>
@@ -15,20 +15,21 @@
     <sheet name="bundles4" sheetId="20" r:id="rId5"/>
     <sheet name="bundles5" sheetId="21" r:id="rId6"/>
     <sheet name="bundles6" sheetId="22" r:id="rId7"/>
-    <sheet name="nthRoot3" sheetId="1" r:id="rId8"/>
-    <sheet name="nthRoot3-2" sheetId="18" r:id="rId9"/>
-    <sheet name="nthRoot4" sheetId="2" r:id="rId10"/>
-    <sheet name="nthRoot4-2" sheetId="11" r:id="rId11"/>
-    <sheet name="nthRoot5-1" sheetId="19" r:id="rId12"/>
-    <sheet name="nthRoot2-4" sheetId="10" r:id="rId13"/>
-    <sheet name="nthRoot9" sheetId="3" r:id="rId14"/>
-    <sheet name="nthRoot9-2" sheetId="4" r:id="rId15"/>
-    <sheet name="precision-1" sheetId="5" r:id="rId16"/>
-    <sheet name="precision-2" sheetId="6" r:id="rId17"/>
-    <sheet name="precision-3" sheetId="7" r:id="rId18"/>
-    <sheet name="precision-4" sheetId="8" r:id="rId19"/>
-    <sheet name="precision-5" sheetId="9" r:id="rId20"/>
-    <sheet name="precision-6" sheetId="13" r:id="rId21"/>
+    <sheet name="bundles7" sheetId="23" r:id="rId8"/>
+    <sheet name="nthRoot3" sheetId="1" r:id="rId9"/>
+    <sheet name="nthRoot3-2" sheetId="18" r:id="rId10"/>
+    <sheet name="nthRoot4" sheetId="2" r:id="rId11"/>
+    <sheet name="nthRoot4-2" sheetId="11" r:id="rId12"/>
+    <sheet name="nthRoot5-1" sheetId="19" r:id="rId13"/>
+    <sheet name="nthRoot2-4" sheetId="10" r:id="rId14"/>
+    <sheet name="nthRoot9" sheetId="3" r:id="rId15"/>
+    <sheet name="nthRoot9-2" sheetId="4" r:id="rId16"/>
+    <sheet name="precision-1" sheetId="5" r:id="rId17"/>
+    <sheet name="precision-2" sheetId="6" r:id="rId18"/>
+    <sheet name="precision-3" sheetId="7" r:id="rId19"/>
+    <sheet name="precision-4" sheetId="8" r:id="rId20"/>
+    <sheet name="precision-5" sheetId="9" r:id="rId21"/>
+    <sheet name="precision-6" sheetId="13" r:id="rId22"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="174">
   <si>
     <t>Largest Multiple of nth root less than or equal to magnitude</t>
   </si>
@@ -550,6 +551,18 @@
   </si>
   <si>
     <t>expectedNthRootDelta</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>X20020</t>
+  </si>
+  <si>
+    <t>expectedActualDelta vs NthRoot</t>
+  </si>
+  <si>
+    <t>expectedActualDelta - NthRoot</t>
   </si>
 </sst>
 </file>
@@ -701,7 +714,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -788,14 +801,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1127,8 +1149,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
       <c r="U1" s="25"/>
       <c r="V1" s="25"/>
     </row>
@@ -2097,6 +2119,778 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386B31B5-45E2-49C7-813A-756A8E1563AE}">
+  <dimension ref="C3:T82"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D3" s="8">
+        <v>98327654.122999996</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D4" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D5" s="1">
+        <v>123</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="3">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D12" s="3">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D13" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D16" s="1">
+        <v>98327654</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="T16" s="3">
+        <f>QUOTIENT(D17,$D$6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D17" s="3">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="T17" s="3">
+        <f>$D$6*T16</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D18" s="3">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="T18" s="1">
+        <f>POWER(10,T17)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D19" s="3">
+        <f>+T19</f>
+        <v>98</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T19" s="3">
+        <f>QUOTIENT(D16,T18)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D21" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D22" s="1">
+        <v>327654</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="T22" s="3">
+        <f>QUOTIENT(D23,$D$6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="T23" s="3">
+        <f>$D$6*T22</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N24" s="12"/>
+      <c r="T24" s="1">
+        <f>POWER(10,T23)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D25" s="3">
+        <f>+T25</f>
+        <v>327</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T25" s="3">
+        <f>QUOTIENT(D22,T24)</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D27" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D28" s="1">
+        <v>654</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="T28" s="3">
+        <f>QUOTIENT(D29,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="T29" s="3">
+        <f>$D$6*T28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="T30" s="1">
+        <f>POWER(10,T29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D31" s="3">
+        <f>+T31</f>
+        <v>654</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T31" s="3">
+        <f>QUOTIENT(D28,T30)</f>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C33" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="35" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D35" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D36" s="1">
+        <v>123</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="T36" s="3">
+        <f>QUOTIENT(D37,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="T37" s="3">
+        <f>$D$6*T36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D38" s="3">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="T38" s="1">
+        <f>POWER(10,T37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D39" s="3">
+        <f>+T39</f>
+        <v>123</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T39" s="3">
+        <f>QUOTIENT(D36,T38)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D44" s="43">
+        <v>98000054.000012293</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D45" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D46" s="1">
+        <v>123</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D48" s="3">
+        <v>7</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D49" s="3">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D52" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D53" s="3">
+        <v>7</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D54" s="3">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D56" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D57" s="1">
+        <v>98000054</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N57" s="3"/>
+      <c r="T57" s="3">
+        <f>QUOTIENT(D58,$D$6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D58" s="3">
+        <v>7</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N58" s="3"/>
+      <c r="T58" s="3">
+        <f>$D$6*T57</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D59" s="3">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N59" s="12"/>
+      <c r="T59" s="1">
+        <f>POWER(10,T58)</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="60" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D60" s="3">
+        <f>+T60</f>
+        <v>98</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T60" s="3">
+        <f>QUOTIENT(D57,T59)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D62" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D63" s="1">
+        <v>54</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="T63" s="1">
+        <f>+D65+D64</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D64" s="1">
+        <v>4</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N64" s="3"/>
+      <c r="T64" s="3">
+        <f>QUOTIENT(D65,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N65" s="3"/>
+      <c r="T65" s="3">
+        <f>$D$6*T64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D66" s="3">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N66" s="12"/>
+      <c r="T66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D69" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D70" s="1">
+        <v>54</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D71" s="1">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N71" s="3"/>
+      <c r="T71" s="3">
+        <f>QUOTIENT(D72,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D72" s="3">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N72" s="3"/>
+      <c r="T72" s="3">
+        <f>$D$6*T71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D73" s="3">
+        <v>3</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N73" s="12"/>
+      <c r="T73" s="1">
+        <f>POWER(10,T72)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D74" s="3">
+        <f>+T74</f>
+        <v>54</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T74" s="3">
+        <f>QUOTIENT(D70,T73)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C76" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="78" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D78" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D79" s="1">
+        <v>123</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N79" s="3"/>
+      <c r="T79" s="3">
+        <f>QUOTIENT(D80,$D$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D80" s="3">
+        <v>2</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N80" s="3"/>
+      <c r="T80" s="3">
+        <f>$D$6*T79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D81" s="3">
+        <v>3</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N81" s="12"/>
+      <c r="T81" s="1">
+        <f>POWER(10,T80)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D82" s="3">
+        <f>+T82</f>
+        <v>123</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T82" s="3">
+        <f>QUOTIENT(D79,T81)</f>
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A7253D-47AB-4549-AA1B-96639CB1F79F}">
   <dimension ref="D3:L16"/>
   <sheetViews>
@@ -2246,7 +3040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC11DC1B-2CEC-4FBC-ADD7-73CA61C21010}">
   <dimension ref="D3:L16"/>
   <sheetViews>
@@ -2396,7 +3190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE433CDA-DA93-4ADC-87D0-0C6CD5FAD8A2}">
   <dimension ref="C3:T84"/>
   <sheetViews>
@@ -3194,7 +3988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03409A07-B58B-490F-BED8-8C6B21724E03}">
   <dimension ref="C3:E14"/>
   <sheetViews>
@@ -3282,7 +4076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDAB58E-8FDE-41DE-BD0D-5DD08E2884E4}">
   <dimension ref="C3:D14"/>
   <sheetViews>
@@ -3388,7 +4182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7C97A5-19D5-400D-884D-AC3B02725D6F}">
   <dimension ref="C3:E14"/>
   <sheetViews>
@@ -3477,7 +4271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F5DF80-EF70-4B4D-A7D6-0733E2C43353}">
   <dimension ref="E3:Q17"/>
   <sheetViews>
@@ -3684,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C28F389-1331-4051-83F6-10A5A26D1AF9}">
   <dimension ref="C2:O16"/>
   <sheetViews>
@@ -3902,7 +4696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104113D6-5DBA-41D8-9C7E-09EB1EAA3D3E}">
   <dimension ref="C2:P16"/>
   <sheetViews>
@@ -4133,237 +4927,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38E82AD-C86B-4FB6-B5D0-72FCD37FF65F}">
-  <dimension ref="C2:Q16"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C2" s="8">
-        <v>98327.123000000007</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C3" s="1">
-        <v>983271230</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="1">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C6" s="3">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C7" s="3">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C8" s="3">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3">
-        <v>3</v>
-      </c>
-      <c r="J11" s="3">
-        <v>4</v>
-      </c>
-      <c r="K11" s="3">
-        <v>5</v>
-      </c>
-      <c r="L11" s="3">
-        <v>6</v>
-      </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3">
-        <v>983271230</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="N12" s="10"/>
-    </row>
-    <row r="14" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3">
-        <v>3</v>
-      </c>
-      <c r="J15" s="3">
-        <v>4</v>
-      </c>
-      <c r="K15" s="3">
-        <v>5</v>
-      </c>
-      <c r="L15" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C16" s="11"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3">
-        <v>3</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="3">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3">
-        <v>8</v>
-      </c>
-      <c r="I16" s="3">
-        <v>7</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
-        <v>8</v>
-      </c>
-      <c r="L16" s="3">
-        <v>3</v>
-      </c>
-      <c r="M16" s="3"/>
-      <c r="O16" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6228,6 +6791,237 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38E82AD-C86B-4FB6-B5D0-72FCD37FF65F}">
+  <dimension ref="C2:Q16"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C2" s="8">
+        <v>98327.123000000007</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="1">
+        <v>983271230</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C8" s="3">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>4</v>
+      </c>
+      <c r="K11" s="3">
+        <v>5</v>
+      </c>
+      <c r="L11" s="3">
+        <v>6</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>983271230</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="14" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4</v>
+      </c>
+      <c r="K15" s="3">
+        <v>5</v>
+      </c>
+      <c r="L15" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="11"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3">
+        <v>7</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>8</v>
+      </c>
+      <c r="L16" s="3">
+        <v>3</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="O16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1CD97A-6BF1-46E9-B4A0-3A5C60052C42}">
   <dimension ref="C2:S17"/>
   <sheetViews>
@@ -6460,7 +7254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0DCCEE-B346-4930-A2C9-A289DE597159}">
   <dimension ref="C2:S18"/>
   <sheetViews>
@@ -8592,10 +9386,10 @@
       <c r="F9" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="J9" s="48"/>
+      <c r="J9" s="47"/>
       <c r="L9" s="3" t="s">
         <v>143</v>
       </c>
@@ -9212,7 +10006,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="47" t="s">
+      <c r="I35" s="46" t="s">
         <v>125</v>
       </c>
       <c r="J35" s="15"/>
@@ -9576,20 +10370,20 @@
       <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50" t="s">
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49" t="s">
         <v>167</v>
       </c>
       <c r="J16" s="17"/>
@@ -9607,7 +10401,7 @@
       <c r="A17" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>149</v>
       </c>
       <c r="C17" s="15">
@@ -9785,20 +10579,20 @@
       <c r="Q23" s="15"/>
     </row>
     <row r="24" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50" t="s">
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50" t="s">
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49" t="s">
         <v>165</v>
       </c>
       <c r="J24" s="15"/>
@@ -10049,7 +10843,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="47" t="s">
+      <c r="I35" s="46" t="s">
         <v>125</v>
       </c>
       <c r="J35" s="15"/>
@@ -10153,10 +10947,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE44156-DA3A-4069-9065-D0B9AA3D46B7}">
-  <dimension ref="A2:S41"/>
+  <dimension ref="A2:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10412,20 +11206,20 @@
       <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50" t="s">
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49" t="s">
         <v>165</v>
       </c>
       <c r="J16" s="17"/>
@@ -10443,7 +11237,7 @@
       <c r="A17" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>149</v>
       </c>
       <c r="C17" s="15">
@@ -10475,17 +11269,34 @@
       <c r="Q17" s="15"/>
     </row>
     <row r="18" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="15">
+        <f>+C17-$C$3</f>
+        <v>-2</v>
+      </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="15">
+        <f>+F17-$C$3</f>
+        <v>1</v>
+      </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="15">
+        <f>+I17-$C$3</f>
+        <v>-1</v>
+      </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="L18" s="15">
+        <f>+L17-$C$3</f>
+        <v>-2</v>
+      </c>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
@@ -10493,22 +11304,14 @@
       <c r="Q18" s="15"/>
     </row>
     <row r="19" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="15">
-        <v>1</v>
-      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="15">
-        <v>1</v>
-      </c>
+      <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="15">
-        <v>1</v>
-      </c>
+      <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
@@ -10520,20 +11323,20 @@
     </row>
     <row r="20" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C20" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
@@ -10546,23 +11349,20 @@
     </row>
     <row r="21" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="15">
-        <f>+C23</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15">
-        <f>+F23</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15">
-        <f>+I23</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -10574,14 +11374,25 @@
       <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="15">
+        <f>+C24</f>
+        <v>4</v>
+      </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="15">
+        <f>+F24</f>
+        <v>4</v>
+      </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="15">
+        <f>+I24</f>
+        <v>4</v>
+      </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
@@ -10592,28 +11403,14 @@
       <c r="Q22" s="15"/>
     </row>
     <row r="23" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C23" s="15">
-        <f>+C20-$C$3</f>
-        <v>4</v>
-      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="15">
-        <f>+F20-$C$3</f>
-        <v>4</v>
-      </c>
+      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
-      <c r="I23" s="15">
-        <f>+I20-$C$3</f>
-        <v>4</v>
-      </c>
+      <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -10624,21 +11421,27 @@
       <c r="Q23" s="15"/>
     </row>
     <row r="24" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B24" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="C24" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50" t="s">
-        <v>165</v>
+      <c r="A24" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="15">
+        <f>+C21-$C$3</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15">
+        <f>+F21-$C$3</f>
+        <v>4</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15">
+        <f>+I21-$C$3</f>
+        <v>4</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
@@ -10650,27 +11453,21 @@
       <c r="Q24" s="15"/>
     </row>
     <row r="25" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C25" s="15">
-        <f>+C20-C19</f>
-        <v>5</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15">
-        <f>+F20-F19</f>
-        <v>5</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15">
-        <f>+I20-I19</f>
-        <v>5</v>
+      <c r="B25" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49" t="s">
+        <v>165</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
@@ -10682,15 +11479,28 @@
       <c r="Q25" s="15"/>
     </row>
     <row r="26" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
+      <c r="A26" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="15">
+        <f>+C21-C20</f>
+        <v>5</v>
+      </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="15">
+        <f>+F21-F20</f>
+        <v>5</v>
+      </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="15">
+        <f>+I21-I20</f>
+        <v>5</v>
+      </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
@@ -10701,22 +11511,15 @@
       <c r="Q26" s="15"/>
     </row>
     <row r="27" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B27" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="15">
-        <v>200000</v>
-      </c>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="15">
-        <v>0</v>
-      </c>
+      <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="15">
-        <v>0</v>
-      </c>
+      <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
@@ -10728,20 +11531,20 @@
     </row>
     <row r="28" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B28" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C28" s="15">
-        <v>5</v>
+        <v>200000</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
@@ -10754,20 +11557,20 @@
     </row>
     <row r="29" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B29" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" s="15">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
@@ -10780,10 +11583,10 @@
     </row>
     <row r="30" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B30" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C30" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -10806,20 +11609,20 @@
     </row>
     <row r="31" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
@@ -10831,13 +11634,22 @@
       <c r="Q31" s="15"/>
     </row>
     <row r="32" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C32" s="15"/>
+      <c r="B32" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="15">
+        <v>5</v>
+      </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="F32" s="15">
+        <v>5</v>
+      </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="I32" s="15">
+        <v>5</v>
+      </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
@@ -10848,12 +11660,7 @@
       <c r="Q32" s="15"/>
     </row>
     <row r="33" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B33" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -10871,14 +11678,14 @@
     </row>
     <row r="34" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B34" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="15"/>
+        <v>159</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>125</v>
+      </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
@@ -10893,12 +11700,14 @@
     </row>
     <row r="35" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B35" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="F35" s="15" t="s">
+        <v>125</v>
+      </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
@@ -10913,7 +11722,7 @@
     </row>
     <row r="36" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B36" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
@@ -10921,9 +11730,7 @@
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="47" t="s">
-        <v>125</v>
-      </c>
+      <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
@@ -10934,13 +11741,18 @@
       <c r="Q36" s="15"/>
     </row>
     <row r="37" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B37" s="15" t="s">
+        <v>162</v>
+      </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
+      <c r="I37" s="46" t="s">
+        <v>125</v>
+      </c>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
@@ -11018,6 +11830,23 @@
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
     </row>
+    <row r="42" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11025,6 +11854,931 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BE6DBA-2355-4186-AC9E-857519730D8C}">
+  <dimension ref="A1:S42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="46.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2020020</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1010205</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="36"/>
+    </row>
+    <row r="5" spans="1:19" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="51"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B11" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="15">
+        <v>7</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15">
+        <v>5</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
+        <v>1</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+    </row>
+    <row r="12" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B12" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="15">
+        <v>7</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15">
+        <v>6</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
+        <v>2</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15">
+        <v>1</v>
+      </c>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+    </row>
+    <row r="13" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B13" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="15">
+        <f>+C15</f>
+        <v>5</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15">
+        <f>+F15</f>
+        <v>4</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15">
+        <f>+I15</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15">
+        <f>+L15</f>
+        <v>-1</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+    </row>
+    <row r="14" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+    </row>
+    <row r="15" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+C12-$C$3</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15">
+        <f>+F12-$C$3</f>
+        <v>4</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15">
+        <f>+I12-$C$3</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15">
+        <f>+L12-$C$3</f>
+        <v>-1</v>
+      </c>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+    </row>
+    <row r="16" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B16" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+    </row>
+    <row r="17" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="15">
+        <f>+C12-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15">
+        <f>+F12-F11</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15">
+        <f>+I12-I11</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15">
+        <f>+L12-L11</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="15">
+        <f>+C17-$C$3</f>
+        <v>-2</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15">
+        <f>+F17-$C$3</f>
+        <v>-1</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15">
+        <f>+I17-$C$3</f>
+        <v>-1</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15">
+        <f>+L17-$C$3</f>
+        <v>-2</v>
+      </c>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+    </row>
+    <row r="19" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+    </row>
+    <row r="20" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B20" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="15">
+        <v>8</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15">
+        <v>8</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15">
+        <v>1</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+    </row>
+    <row r="21" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B21" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="15">
+        <v>8</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15">
+        <v>8</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15">
+        <v>6</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B22" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="15">
+        <f>+C24</f>
+        <v>6</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15">
+        <f>+F24</f>
+        <v>6</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15">
+        <f>+I24</f>
+        <v>4</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+    </row>
+    <row r="24" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="15">
+        <f>+C21-$C$3</f>
+        <v>6</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15">
+        <f>+F21-$C$3</f>
+        <v>6</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15">
+        <f>+I21-$C$3</f>
+        <v>4</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+    </row>
+    <row r="25" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B25" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="15">
+        <f>+C21-C20</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15">
+        <f>+F21-F20</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15">
+        <f>+I21-I20</f>
+        <v>5</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+    </row>
+    <row r="27" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B28" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="15">
+        <v>2020020</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15">
+        <v>0</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B29" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="15">
+        <v>10102050</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15">
+        <v>10102050</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15">
+        <v>5</v>
+      </c>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+    </row>
+    <row r="30" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B30" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="15">
+        <v>2</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15">
+        <v>2</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15">
+        <v>0</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+    </row>
+    <row r="31" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B31" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="15">
+        <v>20020</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15">
+        <v>2</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15">
+        <v>0</v>
+      </c>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+    </row>
+    <row r="32" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B32" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="15">
+        <v>10102050</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15">
+        <f>+F29</f>
+        <v>10102050</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15">
+        <v>5</v>
+      </c>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+    </row>
+    <row r="33" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+    </row>
+    <row r="34" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B34" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+    </row>
+    <row r="35" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B35" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+    </row>
+    <row r="36" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B36" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+    </row>
+    <row r="37" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B37" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+    </row>
+    <row r="38" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+    </row>
+    <row r="39" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+    </row>
+    <row r="40" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+    </row>
+    <row r="41" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+    </row>
+    <row r="42" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F10:G10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D6:O27"/>
   <sheetViews>
@@ -11218,776 +12972,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386B31B5-45E2-49C7-813A-756A8E1563AE}">
-  <dimension ref="C3:T82"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D3" s="8">
-        <v>98327654.122999996</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D4" s="1">
-        <v>98327654</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D5" s="1">
-        <v>123</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D8" s="3">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C10" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D11" s="1">
-        <v>98327654</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D12" s="3">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D13" s="3">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D16" s="1">
-        <v>98327654</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="T16" s="3">
-        <f>QUOTIENT(D17,$D$6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D17" s="3">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="T17" s="3">
-        <f>$D$6*T16</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D18" s="3">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N18" s="12"/>
-      <c r="T18" s="1">
-        <f>POWER(10,T17)</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="19" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D19" s="3">
-        <f>+T19</f>
-        <v>98</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T19" s="3">
-        <f>QUOTIENT(D16,T18)</f>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D21" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D22" s="1">
-        <v>327654</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N22" s="3"/>
-      <c r="T22" s="3">
-        <f>QUOTIENT(D23,$D$6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D23" s="3">
-        <v>5</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N23" s="3"/>
-      <c r="T23" s="3">
-        <f>$D$6*T22</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D24" s="3">
-        <v>6</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N24" s="12"/>
-      <c r="T24" s="1">
-        <f>POWER(10,T23)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D25" s="3">
-        <f>+T25</f>
-        <v>327</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T25" s="3">
-        <f>QUOTIENT(D22,T24)</f>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D27" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D28" s="1">
-        <v>654</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N28" s="3"/>
-      <c r="T28" s="3">
-        <f>QUOTIENT(D29,$D$6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D29" s="3">
-        <v>2</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N29" s="3"/>
-      <c r="T29" s="3">
-        <f>$D$6*T28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D30" s="3">
-        <v>3</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N30" s="12"/>
-      <c r="T30" s="1">
-        <f>POWER(10,T29)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D31" s="3">
-        <f>+T31</f>
-        <v>654</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T31" s="3">
-        <f>QUOTIENT(D28,T30)</f>
-        <v>654</v>
-      </c>
-    </row>
-    <row r="33" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C33" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="35" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D35" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D36" s="1">
-        <v>123</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N36" s="3"/>
-      <c r="T36" s="3">
-        <f>QUOTIENT(D37,$D$6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D37" s="3">
-        <v>2</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N37" s="3"/>
-      <c r="T37" s="3">
-        <f>$D$6*T36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D38" s="3">
-        <v>3</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N38" s="12"/>
-      <c r="T38" s="1">
-        <f>POWER(10,T37)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D39" s="3">
-        <f>+T39</f>
-        <v>123</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T39" s="3">
-        <f>QUOTIENT(D36,T38)</f>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D44" s="43">
-        <v>98000054.000012293</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D45" s="1">
-        <v>98000054</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D46" s="1">
-        <v>123</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D47" s="1">
-        <v>3</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D48" s="3">
-        <v>7</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D49" s="3">
-        <v>7</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C51" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D52" s="1">
-        <v>98000054</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D53" s="3">
-        <v>7</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D54" s="3">
-        <v>8</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D56" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D57" s="1">
-        <v>98000054</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N57" s="3"/>
-      <c r="T57" s="3">
-        <f>QUOTIENT(D58,$D$6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D58" s="3">
-        <v>7</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N58" s="3"/>
-      <c r="T58" s="3">
-        <f>$D$6*T57</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D59" s="3">
-        <v>8</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N59" s="12"/>
-      <c r="T59" s="1">
-        <f>POWER(10,T58)</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="60" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D60" s="3">
-        <f>+T60</f>
-        <v>98</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T60" s="3">
-        <f>QUOTIENT(D57,T59)</f>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D62" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D63" s="1">
-        <v>54</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="T63" s="1">
-        <f>+D65+D64</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D64" s="1">
-        <v>4</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N64" s="3"/>
-      <c r="T64" s="3">
-        <f>QUOTIENT(D65,$D$6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D65" s="3">
-        <v>1</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N65" s="3"/>
-      <c r="T65" s="3">
-        <f>$D$6*T64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D66" s="3">
-        <v>2</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N66" s="12"/>
-      <c r="T66" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D67" s="3">
-        <v>0</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T67" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D69" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D70" s="1">
-        <v>54</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D71" s="1">
-        <v>1</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N71" s="3"/>
-      <c r="T71" s="3">
-        <f>QUOTIENT(D72,$D$6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D72" s="3">
-        <v>2</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N72" s="3"/>
-      <c r="T72" s="3">
-        <f>$D$6*T71</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D73" s="3">
-        <v>3</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N73" s="12"/>
-      <c r="T73" s="1">
-        <f>POWER(10,T72)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D74" s="3">
-        <f>+T74</f>
-        <v>54</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T74" s="3">
-        <f>QUOTIENT(D70,T73)</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C76" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-    </row>
-    <row r="78" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D78" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D79" s="1">
-        <v>123</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L79" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="N79" s="3"/>
-      <c r="T79" s="3">
-        <f>QUOTIENT(D80,$D$6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="3:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D80" s="3">
-        <v>2</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L80" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N80" s="3"/>
-      <c r="T80" s="3">
-        <f>$D$6*T79</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D81" s="3">
-        <v>3</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="N81" s="12"/>
-      <c r="T81" s="1">
-        <f>POWER(10,T80)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="4:20" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="D82" s="3">
-        <f>+T82</f>
-        <v>123</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T82" s="3">
-        <f>QUOTIENT(D79,T81)</f>
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>